<commit_message>
Changes to add age measures
1. Changes to cube add age  measures for Warranty, Outstanding Credits, Cash Outstanding, Work In Progress
2. Changes to power bi report to reports for Warranty, Outstanding Credits, Cash Outstanding, Work In Progress
</commit_message>
<xml_diff>
--- a/All Extracts.xlsx
+++ b/All Extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vamsi\Scania\src\Scania-KPI-Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vamsi\Scania\src\Scania-KPI-Dashboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Dimensions" sheetId="3" r:id="rId3"/>
     <sheet name="Facts" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="522">
   <si>
     <t>Budget</t>
   </si>
@@ -1610,6 +1610,9 @@
   </si>
   <si>
     <t>fact.OutstandingCredit</t>
+  </si>
+  <si>
+    <t>Date In</t>
   </si>
 </sst>
 </file>
@@ -2007,15 +2010,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2033,6 +2027,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3094,18 +3097,18 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41" t="s">
         <v>378</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3135,16 +3138,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3599,18 +3602,18 @@
       <c r="B29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
@@ -3639,16 +3642,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="44" t="s">
         <v>446</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="str">
@@ -3822,18 +3825,18 @@
       <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="44" t="s">
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="46"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="43"/>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
@@ -3862,16 +3865,16 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="str">
@@ -4161,18 +4164,18 @@
     </row>
     <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="44" t="s">
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="46"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="43"/>
     </row>
     <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
@@ -4201,16 +4204,16 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="44" t="s">
         <v>445</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="46"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="str">
@@ -4635,18 +4638,18 @@
     </row>
     <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="44" t="s">
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F81" s="45"/>
-      <c r="G81" s="45"/>
-      <c r="H81" s="46"/>
+      <c r="F81" s="42"/>
+      <c r="G81" s="42"/>
+      <c r="H81" s="43"/>
     </row>
     <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
@@ -4675,16 +4678,16 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="38" t="s">
+      <c r="A83" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
+      <c r="B83" s="45"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="46"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="str">
@@ -4867,18 +4870,18 @@
     </row>
     <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="41" t="s">
+      <c r="A92" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B92" s="42"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="44" t="s">
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="F92" s="45"/>
-      <c r="G92" s="45"/>
-      <c r="H92" s="46"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="42"/>
+      <c r="H92" s="43"/>
     </row>
     <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
@@ -4907,14 +4910,14 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="38"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="40"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="45"/>
+      <c r="C94" s="45"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="45"/>
+      <c r="F94" s="45"/>
+      <c r="G94" s="45"/>
+      <c r="H94" s="46"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="21" t="str">
@@ -5125,18 +5128,18 @@
     </row>
     <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="106" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="B106" s="42"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="43"/>
-      <c r="E106" s="44" t="s">
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F106" s="45"/>
-      <c r="G106" s="45"/>
-      <c r="H106" s="46"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="43"/>
     </row>
     <row r="107" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="13" t="s">
@@ -5165,16 +5168,16 @@
       </c>
     </row>
     <row r="108" spans="1:8" s="12" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="38" t="s">
+      <c r="A108" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="40"/>
+      <c r="B108" s="45"/>
+      <c r="C108" s="45"/>
+      <c r="D108" s="45"/>
+      <c r="E108" s="45"/>
+      <c r="F108" s="45"/>
+      <c r="G108" s="45"/>
+      <c r="H108" s="46"/>
     </row>
     <row r="109" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="21" t="str">
@@ -5340,18 +5343,18 @@
     </row>
     <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="41" t="s">
+      <c r="A117" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="B117" s="42"/>
-      <c r="C117" s="42"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="44" t="s">
+      <c r="B117" s="39"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="40"/>
+      <c r="E117" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="F117" s="45"/>
-      <c r="G117" s="45"/>
-      <c r="H117" s="46"/>
+      <c r="F117" s="42"/>
+      <c r="G117" s="42"/>
+      <c r="H117" s="43"/>
     </row>
     <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
@@ -5380,14 +5383,14 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="38"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="40"/>
+      <c r="A119" s="44"/>
+      <c r="B119" s="45"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="45"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="46"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="21" t="str">
@@ -5501,18 +5504,18 @@
     </row>
     <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="126" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B126" s="42"/>
-      <c r="C126" s="42"/>
-      <c r="D126" s="43"/>
-      <c r="E126" s="44" t="s">
+      <c r="B126" s="39"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="40"/>
+      <c r="E126" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="F126" s="45"/>
-      <c r="G126" s="45"/>
-      <c r="H126" s="46"/>
+      <c r="F126" s="42"/>
+      <c r="G126" s="42"/>
+      <c r="H126" s="43"/>
     </row>
     <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
@@ -5541,14 +5544,14 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="38"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="39"/>
-      <c r="E128" s="39"/>
-      <c r="F128" s="39"/>
-      <c r="G128" s="39"/>
-      <c r="H128" s="40"/>
+      <c r="A128" s="44"/>
+      <c r="B128" s="45"/>
+      <c r="C128" s="45"/>
+      <c r="D128" s="45"/>
+      <c r="E128" s="45"/>
+      <c r="F128" s="45"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="46"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="str">
@@ -5666,18 +5669,18 @@
     </row>
     <row r="134" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="135" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="41" t="s">
+      <c r="A135" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="B135" s="42"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="43"/>
-      <c r="E135" s="44" t="s">
+      <c r="B135" s="39"/>
+      <c r="C135" s="39"/>
+      <c r="D135" s="40"/>
+      <c r="E135" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="F135" s="45"/>
-      <c r="G135" s="45"/>
-      <c r="H135" s="46"/>
+      <c r="F135" s="42"/>
+      <c r="G135" s="42"/>
+      <c r="H135" s="43"/>
     </row>
     <row r="136" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="13" t="s">
@@ -5706,14 +5709,14 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="38"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="39"/>
-      <c r="D137" s="39"/>
-      <c r="E137" s="39"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="39"/>
-      <c r="H137" s="40"/>
+      <c r="A137" s="44"/>
+      <c r="B137" s="45"/>
+      <c r="C137" s="45"/>
+      <c r="D137" s="45"/>
+      <c r="E137" s="45"/>
+      <c r="F137" s="45"/>
+      <c r="G137" s="45"/>
+      <c r="H137" s="46"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="str">
@@ -5836,18 +5839,18 @@
     </row>
     <row r="144" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="145" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="41" t="s">
+      <c r="A145" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="B145" s="42"/>
-      <c r="C145" s="42"/>
-      <c r="D145" s="43"/>
-      <c r="E145" s="44" t="s">
+      <c r="B145" s="39"/>
+      <c r="C145" s="39"/>
+      <c r="D145" s="40"/>
+      <c r="E145" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="F145" s="45"/>
-      <c r="G145" s="45"/>
-      <c r="H145" s="46"/>
+      <c r="F145" s="42"/>
+      <c r="G145" s="42"/>
+      <c r="H145" s="43"/>
     </row>
     <row r="146" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13" t="s">
@@ -5876,16 +5879,16 @@
       </c>
     </row>
     <row r="147" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="38" t="s">
+      <c r="A147" s="44" t="s">
         <v>268</v>
       </c>
-      <c r="B147" s="39"/>
-      <c r="C147" s="39"/>
-      <c r="D147" s="39"/>
-      <c r="E147" s="39"/>
-      <c r="F147" s="39"/>
-      <c r="G147" s="39"/>
-      <c r="H147" s="40"/>
+      <c r="B147" s="45"/>
+      <c r="C147" s="45"/>
+      <c r="D147" s="45"/>
+      <c r="E147" s="45"/>
+      <c r="F147" s="45"/>
+      <c r="G147" s="45"/>
+      <c r="H147" s="46"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="21" t="str">
@@ -6008,18 +6011,18 @@
     </row>
     <row r="153" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="154" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="41" t="s">
+      <c r="A154" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B154" s="42"/>
-      <c r="C154" s="42"/>
-      <c r="D154" s="43"/>
-      <c r="E154" s="44" t="s">
+      <c r="B154" s="39"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="F154" s="45"/>
-      <c r="G154" s="45"/>
-      <c r="H154" s="46"/>
+      <c r="F154" s="42"/>
+      <c r="G154" s="42"/>
+      <c r="H154" s="43"/>
     </row>
     <row r="155" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="13" t="s">
@@ -6048,16 +6051,16 @@
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="38" t="s">
+      <c r="A156" s="44" t="s">
         <v>283</v>
       </c>
-      <c r="B156" s="39"/>
-      <c r="C156" s="39"/>
-      <c r="D156" s="39"/>
-      <c r="E156" s="39"/>
-      <c r="F156" s="39"/>
-      <c r="G156" s="39"/>
-      <c r="H156" s="40"/>
+      <c r="B156" s="45"/>
+      <c r="C156" s="45"/>
+      <c r="D156" s="45"/>
+      <c r="E156" s="45"/>
+      <c r="F156" s="45"/>
+      <c r="G156" s="45"/>
+      <c r="H156" s="46"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="21" t="str">
@@ -6682,24 +6685,15 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="E126:H126"/>
-    <mergeCell ref="A128:H128"/>
-    <mergeCell ref="A108:H108"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="E117:H117"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="A83:H83"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="E92:H92"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="E106:H106"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="E60:H60"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="A147:H147"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="E154:H154"/>
+    <mergeCell ref="A156:H156"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="E135:H135"/>
+    <mergeCell ref="A137:H137"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="E145:H145"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="A30:D30"/>
@@ -6711,15 +6705,24 @@
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A147:H147"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="E154:H154"/>
-    <mergeCell ref="A156:H156"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="E135:H135"/>
-    <mergeCell ref="A137:H137"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="E145:H145"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="E60:H60"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="A83:H83"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="E92:H92"/>
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="E106:H106"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="E126:H126"/>
+    <mergeCell ref="A128:H128"/>
+    <mergeCell ref="A108:H108"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="E117:H117"/>
+    <mergeCell ref="A119:H119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6729,8 +6732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D216" sqref="D216"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6798,18 +6801,18 @@
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
@@ -6838,16 +6841,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="str">
@@ -6992,18 +6995,18 @@
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
@@ -7032,14 +7035,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="str">
@@ -7180,18 +7183,18 @@
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
@@ -7220,16 +7223,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="44" t="s">
         <v>462</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="str">
@@ -7859,18 +7862,18 @@
     </row>
     <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="42"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="44" t="s">
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="F64" s="45"/>
-      <c r="G64" s="45"/>
-      <c r="H64" s="46"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="43"/>
     </row>
     <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
@@ -7899,16 +7902,16 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="46"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="str">
@@ -9034,18 +9037,18 @@
     </row>
     <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="128" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B128" s="42"/>
-      <c r="C128" s="42"/>
-      <c r="D128" s="43"/>
-      <c r="E128" s="44" t="s">
+      <c r="B128" s="39"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="40"/>
+      <c r="E128" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="F128" s="45"/>
-      <c r="G128" s="45"/>
-      <c r="H128" s="46"/>
+      <c r="F128" s="42"/>
+      <c r="G128" s="42"/>
+      <c r="H128" s="43"/>
     </row>
     <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
@@ -9074,14 +9077,14 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="38"/>
-      <c r="B130" s="39"/>
-      <c r="C130" s="39"/>
-      <c r="D130" s="39"/>
-      <c r="E130" s="39"/>
-      <c r="F130" s="39"/>
-      <c r="G130" s="39"/>
-      <c r="H130" s="40"/>
+      <c r="A130" s="44"/>
+      <c r="B130" s="45"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="46"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="str">
@@ -9346,18 +9349,18 @@
     </row>
     <row r="143" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="144" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="41" t="s">
+      <c r="A144" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="B144" s="42"/>
-      <c r="C144" s="42"/>
-      <c r="D144" s="43"/>
-      <c r="E144" s="44" t="s">
+      <c r="B144" s="39"/>
+      <c r="C144" s="39"/>
+      <c r="D144" s="40"/>
+      <c r="E144" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="F144" s="45"/>
-      <c r="G144" s="45"/>
-      <c r="H144" s="46"/>
+      <c r="F144" s="42"/>
+      <c r="G144" s="42"/>
+      <c r="H144" s="43"/>
     </row>
     <row r="145" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="13" t="s">
@@ -9386,14 +9389,14 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="38"/>
-      <c r="B146" s="39"/>
-      <c r="C146" s="39"/>
-      <c r="D146" s="39"/>
-      <c r="E146" s="39"/>
-      <c r="F146" s="39"/>
-      <c r="G146" s="39"/>
-      <c r="H146" s="40"/>
+      <c r="A146" s="44"/>
+      <c r="B146" s="45"/>
+      <c r="C146" s="45"/>
+      <c r="D146" s="45"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="45"/>
+      <c r="G146" s="45"/>
+      <c r="H146" s="46"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="str">
@@ -9678,18 +9681,18 @@
     </row>
     <row r="160" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="161" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="41" t="s">
+      <c r="A161" s="38" t="s">
         <v>520</v>
       </c>
-      <c r="B161" s="42"/>
-      <c r="C161" s="42"/>
-      <c r="D161" s="43"/>
-      <c r="E161" s="44" t="s">
+      <c r="B161" s="39"/>
+      <c r="C161" s="39"/>
+      <c r="D161" s="40"/>
+      <c r="E161" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="F161" s="45"/>
-      <c r="G161" s="45"/>
-      <c r="H161" s="46"/>
+      <c r="F161" s="42"/>
+      <c r="G161" s="42"/>
+      <c r="H161" s="43"/>
     </row>
     <row r="162" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
@@ -9718,16 +9721,16 @@
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" s="38" t="s">
+      <c r="A163" s="44" t="s">
         <v>508</v>
       </c>
-      <c r="B163" s="39"/>
-      <c r="C163" s="39"/>
-      <c r="D163" s="39"/>
-      <c r="E163" s="39"/>
-      <c r="F163" s="39"/>
-      <c r="G163" s="39"/>
-      <c r="H163" s="40"/>
+      <c r="B163" s="45"/>
+      <c r="C163" s="45"/>
+      <c r="D163" s="45"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="45"/>
+      <c r="G163" s="45"/>
+      <c r="H163" s="46"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="17" t="str">
@@ -10079,18 +10082,18 @@
     </row>
     <row r="182" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="183" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="41" t="s">
+      <c r="A183" s="38" t="s">
         <v>506</v>
       </c>
-      <c r="B183" s="42"/>
-      <c r="C183" s="42"/>
-      <c r="D183" s="43"/>
-      <c r="E183" s="44" t="s">
+      <c r="B183" s="39"/>
+      <c r="C183" s="39"/>
+      <c r="D183" s="40"/>
+      <c r="E183" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="F183" s="45"/>
-      <c r="G183" s="45"/>
-      <c r="H183" s="46"/>
+      <c r="F183" s="42"/>
+      <c r="G183" s="42"/>
+      <c r="H183" s="43"/>
     </row>
     <row r="184" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="13" t="s">
@@ -10119,16 +10122,16 @@
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A185" s="38" t="s">
+      <c r="A185" s="44" t="s">
         <v>503</v>
       </c>
-      <c r="B185" s="39"/>
-      <c r="C185" s="39"/>
-      <c r="D185" s="39"/>
-      <c r="E185" s="39"/>
-      <c r="F185" s="39"/>
-      <c r="G185" s="39"/>
-      <c r="H185" s="40"/>
+      <c r="B185" s="45"/>
+      <c r="C185" s="45"/>
+      <c r="D185" s="45"/>
+      <c r="E185" s="45"/>
+      <c r="F185" s="45"/>
+      <c r="G185" s="45"/>
+      <c r="H185" s="46"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="17" t="str">
@@ -10495,18 +10498,18 @@
     </row>
     <row r="204" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="205" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="41" t="s">
+      <c r="A205" s="38" t="s">
         <v>505</v>
       </c>
-      <c r="B205" s="42"/>
-      <c r="C205" s="42"/>
-      <c r="D205" s="43"/>
-      <c r="E205" s="44" t="s">
+      <c r="B205" s="39"/>
+      <c r="C205" s="39"/>
+      <c r="D205" s="40"/>
+      <c r="E205" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="F205" s="45"/>
-      <c r="G205" s="45"/>
-      <c r="H205" s="46"/>
+      <c r="F205" s="42"/>
+      <c r="G205" s="42"/>
+      <c r="H205" s="43"/>
     </row>
     <row r="206" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="13" t="s">
@@ -10535,16 +10538,16 @@
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A207" s="38" t="s">
+      <c r="A207" s="44" t="s">
         <v>513</v>
       </c>
-      <c r="B207" s="39"/>
-      <c r="C207" s="39"/>
-      <c r="D207" s="39"/>
-      <c r="E207" s="39"/>
-      <c r="F207" s="39"/>
-      <c r="G207" s="39"/>
-      <c r="H207" s="40"/>
+      <c r="B207" s="45"/>
+      <c r="C207" s="45"/>
+      <c r="D207" s="45"/>
+      <c r="E207" s="45"/>
+      <c r="F207" s="45"/>
+      <c r="G207" s="45"/>
+      <c r="H207" s="46"/>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="17" t="str">
@@ -10843,18 +10846,18 @@
     </row>
     <row r="222" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="223" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A223" s="41" t="s">
+      <c r="A223" s="38" t="s">
         <v>502</v>
       </c>
-      <c r="B223" s="42"/>
-      <c r="C223" s="42"/>
-      <c r="D223" s="43"/>
-      <c r="E223" s="44" t="s">
+      <c r="B223" s="39"/>
+      <c r="C223" s="39"/>
+      <c r="D223" s="40"/>
+      <c r="E223" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="F223" s="45"/>
-      <c r="G223" s="45"/>
-      <c r="H223" s="46"/>
+      <c r="F223" s="42"/>
+      <c r="G223" s="42"/>
+      <c r="H223" s="43"/>
     </row>
     <row r="224" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A224" s="13" t="s">
@@ -10883,16 +10886,16 @@
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A225" s="38" t="s">
+      <c r="A225" s="44" t="s">
         <v>510</v>
       </c>
-      <c r="B225" s="39"/>
-      <c r="C225" s="39"/>
-      <c r="D225" s="39"/>
-      <c r="E225" s="39"/>
-      <c r="F225" s="39"/>
-      <c r="G225" s="39"/>
-      <c r="H225" s="40"/>
+      <c r="B225" s="45"/>
+      <c r="C225" s="45"/>
+      <c r="D225" s="45"/>
+      <c r="E225" s="45"/>
+      <c r="F225" s="45"/>
+      <c r="G225" s="45"/>
+      <c r="H225" s="46"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="17" t="str">
@@ -11256,18 +11259,18 @@
     </row>
     <row r="242" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="243" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A243" s="41" t="s">
+      <c r="A243" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="B243" s="42"/>
-      <c r="C243" s="42"/>
-      <c r="D243" s="43"/>
-      <c r="E243" s="44" t="s">
+      <c r="B243" s="39"/>
+      <c r="C243" s="39"/>
+      <c r="D243" s="40"/>
+      <c r="E243" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="F243" s="45"/>
-      <c r="G243" s="45"/>
-      <c r="H243" s="46"/>
+      <c r="F243" s="42"/>
+      <c r="G243" s="42"/>
+      <c r="H243" s="43"/>
     </row>
     <row r="244" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A244" s="13" t="s">
@@ -11296,14 +11299,14 @@
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A245" s="38"/>
-      <c r="B245" s="39"/>
-      <c r="C245" s="39"/>
-      <c r="D245" s="39"/>
-      <c r="E245" s="39"/>
-      <c r="F245" s="39"/>
-      <c r="G245" s="39"/>
-      <c r="H245" s="40"/>
+      <c r="A245" s="44"/>
+      <c r="B245" s="45"/>
+      <c r="C245" s="45"/>
+      <c r="D245" s="45"/>
+      <c r="E245" s="45"/>
+      <c r="F245" s="45"/>
+      <c r="G245" s="45"/>
+      <c r="H245" s="46"/>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" s="17" t="str">
@@ -11503,7 +11506,7 @@
         <v>BWS.csv and BWN.csv</v>
       </c>
       <c r="G254" s="17" t="s">
-        <v>254</v>
+        <v>521</v>
       </c>
       <c r="H254" s="17" t="s">
         <v>255</v>
@@ -11527,7 +11530,7 @@
         <v>BWS.csv and BWN.csv</v>
       </c>
       <c r="G255" s="17" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="H255" s="17"/>
     </row>
@@ -11804,22 +11807,15 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="E64:H64"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="E161:H161"/>
-    <mergeCell ref="A163:H163"/>
-    <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="E128:H128"/>
-    <mergeCell ref="A130:H130"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="E144:H144"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A205:D205"/>
+    <mergeCell ref="E205:H205"/>
+    <mergeCell ref="A245:H245"/>
+    <mergeCell ref="A207:H207"/>
+    <mergeCell ref="A223:D223"/>
+    <mergeCell ref="E223:H223"/>
+    <mergeCell ref="A225:H225"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="E243:H243"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="E17:H17"/>
     <mergeCell ref="A183:D183"/>
@@ -11836,15 +11832,22 @@
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A205:D205"/>
-    <mergeCell ref="E205:H205"/>
-    <mergeCell ref="A245:H245"/>
-    <mergeCell ref="A207:H207"/>
-    <mergeCell ref="A223:D223"/>
-    <mergeCell ref="E223:H223"/>
-    <mergeCell ref="A225:H225"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="E243:H243"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="E64:H64"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="E161:H161"/>
+    <mergeCell ref="A163:H163"/>
+    <mergeCell ref="A113:H113"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="E128:H128"/>
+    <mergeCell ref="A130:H130"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="E144:H144"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to obsolesence B99 file, new SGB Tech Hours file, TimeToInvoice file
</commit_message>
<xml_diff>
--- a/All Extracts.xlsx
+++ b/All Extracts.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Dimensions" sheetId="3" r:id="rId3"/>
     <sheet name="Facts" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="521">
   <si>
     <t>Budget</t>
   </si>
@@ -1602,6 +1602,12 @@
   </si>
   <si>
     <t>Branches_20180930</t>
+  </si>
+  <si>
+    <t>BWC</t>
+  </si>
+  <si>
+    <t>Waste Cost</t>
   </si>
 </sst>
 </file>
@@ -1999,15 +2005,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2025,6 +2022,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2349,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G21" sqref="A1:G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,6 +2870,14 @@
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="D26" t="s">
+        <v>520</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3023,18 +3037,18 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3064,16 +3078,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3528,18 +3542,18 @@
       <c r="B29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
@@ -3568,16 +3582,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="str">
@@ -3751,18 +3765,18 @@
       <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="44" t="s">
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="46"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="43"/>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
@@ -3791,16 +3805,16 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="str">
@@ -4090,18 +4104,18 @@
     </row>
     <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="44" t="s">
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="46"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="43"/>
     </row>
     <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
@@ -4130,16 +4144,16 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="46"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="str">
@@ -4564,18 +4578,18 @@
     </row>
     <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="44" t="s">
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F81" s="45"/>
-      <c r="G81" s="45"/>
-      <c r="H81" s="46"/>
+      <c r="F81" s="42"/>
+      <c r="G81" s="42"/>
+      <c r="H81" s="43"/>
     </row>
     <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
@@ -4604,16 +4618,16 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="38" t="s">
+      <c r="A83" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
+      <c r="B83" s="45"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="46"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="str">
@@ -4796,18 +4810,18 @@
     </row>
     <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="41" t="s">
+      <c r="A92" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B92" s="42"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="44" t="s">
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="F92" s="45"/>
-      <c r="G92" s="45"/>
-      <c r="H92" s="46"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="42"/>
+      <c r="H92" s="43"/>
     </row>
     <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
@@ -4836,14 +4850,14 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="38"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="40"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="45"/>
+      <c r="C94" s="45"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="45"/>
+      <c r="F94" s="45"/>
+      <c r="G94" s="45"/>
+      <c r="H94" s="46"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="21" t="str">
@@ -5054,18 +5068,18 @@
     </row>
     <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="106" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="B106" s="42"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="43"/>
-      <c r="E106" s="44" t="s">
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F106" s="45"/>
-      <c r="G106" s="45"/>
-      <c r="H106" s="46"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="43"/>
     </row>
     <row r="107" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="13" t="s">
@@ -5094,16 +5108,16 @@
       </c>
     </row>
     <row r="108" spans="1:8" s="12" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="38" t="s">
+      <c r="A108" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="40"/>
+      <c r="B108" s="45"/>
+      <c r="C108" s="45"/>
+      <c r="D108" s="45"/>
+      <c r="E108" s="45"/>
+      <c r="F108" s="45"/>
+      <c r="G108" s="45"/>
+      <c r="H108" s="46"/>
     </row>
     <row r="109" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="21" t="str">
@@ -5269,18 +5283,18 @@
     </row>
     <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="41" t="s">
+      <c r="A117" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="B117" s="42"/>
-      <c r="C117" s="42"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="44" t="s">
+      <c r="B117" s="39"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="40"/>
+      <c r="E117" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="F117" s="45"/>
-      <c r="G117" s="45"/>
-      <c r="H117" s="46"/>
+      <c r="F117" s="42"/>
+      <c r="G117" s="42"/>
+      <c r="H117" s="43"/>
     </row>
     <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
@@ -5309,14 +5323,14 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="38"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="40"/>
+      <c r="A119" s="44"/>
+      <c r="B119" s="45"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="45"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="46"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="21" t="str">
@@ -5430,18 +5444,18 @@
     </row>
     <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="126" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="B126" s="42"/>
-      <c r="C126" s="42"/>
-      <c r="D126" s="43"/>
-      <c r="E126" s="44" t="s">
+      <c r="B126" s="39"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="40"/>
+      <c r="E126" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="F126" s="45"/>
-      <c r="G126" s="45"/>
-      <c r="H126" s="46"/>
+      <c r="F126" s="42"/>
+      <c r="G126" s="42"/>
+      <c r="H126" s="43"/>
     </row>
     <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
@@ -5470,14 +5484,14 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="38"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="39"/>
-      <c r="E128" s="39"/>
-      <c r="F128" s="39"/>
-      <c r="G128" s="39"/>
-      <c r="H128" s="40"/>
+      <c r="A128" s="44"/>
+      <c r="B128" s="45"/>
+      <c r="C128" s="45"/>
+      <c r="D128" s="45"/>
+      <c r="E128" s="45"/>
+      <c r="F128" s="45"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="46"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="str">
@@ -5595,18 +5609,18 @@
     </row>
     <row r="134" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="135" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="41" t="s">
+      <c r="A135" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="B135" s="42"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="43"/>
-      <c r="E135" s="44" t="s">
+      <c r="B135" s="39"/>
+      <c r="C135" s="39"/>
+      <c r="D135" s="40"/>
+      <c r="E135" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="F135" s="45"/>
-      <c r="G135" s="45"/>
-      <c r="H135" s="46"/>
+      <c r="F135" s="42"/>
+      <c r="G135" s="42"/>
+      <c r="H135" s="43"/>
     </row>
     <row r="136" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="13" t="s">
@@ -5635,14 +5649,14 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="38"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="39"/>
-      <c r="D137" s="39"/>
-      <c r="E137" s="39"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="39"/>
-      <c r="H137" s="40"/>
+      <c r="A137" s="44"/>
+      <c r="B137" s="45"/>
+      <c r="C137" s="45"/>
+      <c r="D137" s="45"/>
+      <c r="E137" s="45"/>
+      <c r="F137" s="45"/>
+      <c r="G137" s="45"/>
+      <c r="H137" s="46"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="str">
@@ -5765,18 +5779,18 @@
     </row>
     <row r="144" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="145" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="41" t="s">
+      <c r="A145" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="B145" s="42"/>
-      <c r="C145" s="42"/>
-      <c r="D145" s="43"/>
-      <c r="E145" s="44" t="s">
+      <c r="B145" s="39"/>
+      <c r="C145" s="39"/>
+      <c r="D145" s="40"/>
+      <c r="E145" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="F145" s="45"/>
-      <c r="G145" s="45"/>
-      <c r="H145" s="46"/>
+      <c r="F145" s="42"/>
+      <c r="G145" s="42"/>
+      <c r="H145" s="43"/>
     </row>
     <row r="146" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13" t="s">
@@ -5805,16 +5819,16 @@
       </c>
     </row>
     <row r="147" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="38" t="s">
+      <c r="A147" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="B147" s="39"/>
-      <c r="C147" s="39"/>
-      <c r="D147" s="39"/>
-      <c r="E147" s="39"/>
-      <c r="F147" s="39"/>
-      <c r="G147" s="39"/>
-      <c r="H147" s="40"/>
+      <c r="B147" s="45"/>
+      <c r="C147" s="45"/>
+      <c r="D147" s="45"/>
+      <c r="E147" s="45"/>
+      <c r="F147" s="45"/>
+      <c r="G147" s="45"/>
+      <c r="H147" s="46"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="21" t="str">
@@ -5937,18 +5951,18 @@
     </row>
     <row r="153" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="154" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="41" t="s">
+      <c r="A154" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B154" s="42"/>
-      <c r="C154" s="42"/>
-      <c r="D154" s="43"/>
-      <c r="E154" s="44" t="s">
+      <c r="B154" s="39"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="F154" s="45"/>
-      <c r="G154" s="45"/>
-      <c r="H154" s="46"/>
+      <c r="F154" s="42"/>
+      <c r="G154" s="42"/>
+      <c r="H154" s="43"/>
     </row>
     <row r="155" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="13" t="s">
@@ -5977,16 +5991,16 @@
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="38" t="s">
+      <c r="A156" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="B156" s="39"/>
-      <c r="C156" s="39"/>
-      <c r="D156" s="39"/>
-      <c r="E156" s="39"/>
-      <c r="F156" s="39"/>
-      <c r="G156" s="39"/>
-      <c r="H156" s="40"/>
+      <c r="B156" s="45"/>
+      <c r="C156" s="45"/>
+      <c r="D156" s="45"/>
+      <c r="E156" s="45"/>
+      <c r="F156" s="45"/>
+      <c r="G156" s="45"/>
+      <c r="H156" s="46"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="21" t="str">
@@ -6611,24 +6625,15 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="E126:H126"/>
-    <mergeCell ref="A128:H128"/>
-    <mergeCell ref="A108:H108"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="E117:H117"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="A83:H83"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="E92:H92"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="E106:H106"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="E60:H60"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="A147:H147"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="E154:H154"/>
+    <mergeCell ref="A156:H156"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="E135:H135"/>
+    <mergeCell ref="A137:H137"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="E145:H145"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="A30:D30"/>
@@ -6640,15 +6645,24 @@
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A147:H147"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="E154:H154"/>
-    <mergeCell ref="A156:H156"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="E135:H135"/>
-    <mergeCell ref="A137:H137"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="E145:H145"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="E60:H60"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="A83:H83"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="E92:H92"/>
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="E106:H106"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="E126:H126"/>
+    <mergeCell ref="A128:H128"/>
+    <mergeCell ref="A108:H108"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="E117:H117"/>
+    <mergeCell ref="A119:H119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6727,18 +6741,18 @@
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
@@ -6767,16 +6781,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="str">
@@ -6921,18 +6935,18 @@
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
@@ -6961,14 +6975,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="str">
@@ -7109,18 +7123,18 @@
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41" t="s">
         <v>316</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
@@ -7149,16 +7163,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="44" t="s">
         <v>452</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="str">
@@ -7788,18 +7802,18 @@
     </row>
     <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="B64" s="42"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="44" t="s">
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="F64" s="45"/>
-      <c r="G64" s="45"/>
-      <c r="H64" s="46"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="43"/>
     </row>
     <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
@@ -7828,16 +7842,16 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="46"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="str">
@@ -8963,18 +8977,18 @@
     </row>
     <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="128" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B128" s="42"/>
-      <c r="C128" s="42"/>
-      <c r="D128" s="43"/>
-      <c r="E128" s="44" t="s">
+      <c r="B128" s="39"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="40"/>
+      <c r="E128" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="F128" s="45"/>
-      <c r="G128" s="45"/>
-      <c r="H128" s="46"/>
+      <c r="F128" s="42"/>
+      <c r="G128" s="42"/>
+      <c r="H128" s="43"/>
     </row>
     <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
@@ -9003,14 +9017,14 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="38"/>
-      <c r="B130" s="39"/>
-      <c r="C130" s="39"/>
-      <c r="D130" s="39"/>
-      <c r="E130" s="39"/>
-      <c r="F130" s="39"/>
-      <c r="G130" s="39"/>
-      <c r="H130" s="40"/>
+      <c r="A130" s="44"/>
+      <c r="B130" s="45"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="46"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="str">
@@ -9275,18 +9289,18 @@
     </row>
     <row r="143" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="144" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="41" t="s">
+      <c r="A144" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B144" s="42"/>
-      <c r="C144" s="42"/>
-      <c r="D144" s="43"/>
-      <c r="E144" s="44" t="s">
+      <c r="B144" s="39"/>
+      <c r="C144" s="39"/>
+      <c r="D144" s="40"/>
+      <c r="E144" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="F144" s="45"/>
-      <c r="G144" s="45"/>
-      <c r="H144" s="46"/>
+      <c r="F144" s="42"/>
+      <c r="G144" s="42"/>
+      <c r="H144" s="43"/>
     </row>
     <row r="145" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="13" t="s">
@@ -9315,14 +9329,14 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="38"/>
-      <c r="B146" s="39"/>
-      <c r="C146" s="39"/>
-      <c r="D146" s="39"/>
-      <c r="E146" s="39"/>
-      <c r="F146" s="39"/>
-      <c r="G146" s="39"/>
-      <c r="H146" s="40"/>
+      <c r="A146" s="44"/>
+      <c r="B146" s="45"/>
+      <c r="C146" s="45"/>
+      <c r="D146" s="45"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="45"/>
+      <c r="G146" s="45"/>
+      <c r="H146" s="46"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="str">
@@ -9607,18 +9621,18 @@
     </row>
     <row r="160" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="161" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="41" t="s">
+      <c r="A161" s="38" t="s">
         <v>510</v>
       </c>
-      <c r="B161" s="42"/>
-      <c r="C161" s="42"/>
-      <c r="D161" s="43"/>
-      <c r="E161" s="44" t="s">
+      <c r="B161" s="39"/>
+      <c r="C161" s="39"/>
+      <c r="D161" s="40"/>
+      <c r="E161" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="F161" s="45"/>
-      <c r="G161" s="45"/>
-      <c r="H161" s="46"/>
+      <c r="F161" s="42"/>
+      <c r="G161" s="42"/>
+      <c r="H161" s="43"/>
     </row>
     <row r="162" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
@@ -9647,16 +9661,16 @@
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" s="38" t="s">
+      <c r="A163" s="44" t="s">
         <v>498</v>
       </c>
-      <c r="B163" s="39"/>
-      <c r="C163" s="39"/>
-      <c r="D163" s="39"/>
-      <c r="E163" s="39"/>
-      <c r="F163" s="39"/>
-      <c r="G163" s="39"/>
-      <c r="H163" s="40"/>
+      <c r="B163" s="45"/>
+      <c r="C163" s="45"/>
+      <c r="D163" s="45"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="45"/>
+      <c r="G163" s="45"/>
+      <c r="H163" s="46"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="17" t="str">
@@ -10008,18 +10022,18 @@
     </row>
     <row r="182" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="183" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="41" t="s">
+      <c r="A183" s="38" t="s">
         <v>496</v>
       </c>
-      <c r="B183" s="42"/>
-      <c r="C183" s="42"/>
-      <c r="D183" s="43"/>
-      <c r="E183" s="44" t="s">
+      <c r="B183" s="39"/>
+      <c r="C183" s="39"/>
+      <c r="D183" s="40"/>
+      <c r="E183" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="F183" s="45"/>
-      <c r="G183" s="45"/>
-      <c r="H183" s="46"/>
+      <c r="F183" s="42"/>
+      <c r="G183" s="42"/>
+      <c r="H183" s="43"/>
     </row>
     <row r="184" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="13" t="s">
@@ -10048,16 +10062,16 @@
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A185" s="38" t="s">
+      <c r="A185" s="44" t="s">
         <v>493</v>
       </c>
-      <c r="B185" s="39"/>
-      <c r="C185" s="39"/>
-      <c r="D185" s="39"/>
-      <c r="E185" s="39"/>
-      <c r="F185" s="39"/>
-      <c r="G185" s="39"/>
-      <c r="H185" s="40"/>
+      <c r="B185" s="45"/>
+      <c r="C185" s="45"/>
+      <c r="D185" s="45"/>
+      <c r="E185" s="45"/>
+      <c r="F185" s="45"/>
+      <c r="G185" s="45"/>
+      <c r="H185" s="46"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="17" t="str">
@@ -10424,18 +10438,18 @@
     </row>
     <row r="204" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="205" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="41" t="s">
+      <c r="A205" s="38" t="s">
         <v>495</v>
       </c>
-      <c r="B205" s="42"/>
-      <c r="C205" s="42"/>
-      <c r="D205" s="43"/>
-      <c r="E205" s="44" t="s">
+      <c r="B205" s="39"/>
+      <c r="C205" s="39"/>
+      <c r="D205" s="40"/>
+      <c r="E205" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="F205" s="45"/>
-      <c r="G205" s="45"/>
-      <c r="H205" s="46"/>
+      <c r="F205" s="42"/>
+      <c r="G205" s="42"/>
+      <c r="H205" s="43"/>
     </row>
     <row r="206" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="13" t="s">
@@ -10464,16 +10478,16 @@
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A207" s="38" t="s">
+      <c r="A207" s="44" t="s">
         <v>503</v>
       </c>
-      <c r="B207" s="39"/>
-      <c r="C207" s="39"/>
-      <c r="D207" s="39"/>
-      <c r="E207" s="39"/>
-      <c r="F207" s="39"/>
-      <c r="G207" s="39"/>
-      <c r="H207" s="40"/>
+      <c r="B207" s="45"/>
+      <c r="C207" s="45"/>
+      <c r="D207" s="45"/>
+      <c r="E207" s="45"/>
+      <c r="F207" s="45"/>
+      <c r="G207" s="45"/>
+      <c r="H207" s="46"/>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="17" t="str">
@@ -10772,18 +10786,18 @@
     </row>
     <row r="222" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="223" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A223" s="41" t="s">
+      <c r="A223" s="38" t="s">
         <v>492</v>
       </c>
-      <c r="B223" s="42"/>
-      <c r="C223" s="42"/>
-      <c r="D223" s="43"/>
-      <c r="E223" s="44" t="s">
+      <c r="B223" s="39"/>
+      <c r="C223" s="39"/>
+      <c r="D223" s="40"/>
+      <c r="E223" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="F223" s="45"/>
-      <c r="G223" s="45"/>
-      <c r="H223" s="46"/>
+      <c r="F223" s="42"/>
+      <c r="G223" s="42"/>
+      <c r="H223" s="43"/>
     </row>
     <row r="224" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A224" s="13" t="s">
@@ -10812,16 +10826,16 @@
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A225" s="38" t="s">
+      <c r="A225" s="44" t="s">
         <v>500</v>
       </c>
-      <c r="B225" s="39"/>
-      <c r="C225" s="39"/>
-      <c r="D225" s="39"/>
-      <c r="E225" s="39"/>
-      <c r="F225" s="39"/>
-      <c r="G225" s="39"/>
-      <c r="H225" s="40"/>
+      <c r="B225" s="45"/>
+      <c r="C225" s="45"/>
+      <c r="D225" s="45"/>
+      <c r="E225" s="45"/>
+      <c r="F225" s="45"/>
+      <c r="G225" s="45"/>
+      <c r="H225" s="46"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="17" t="str">
@@ -11185,18 +11199,18 @@
     </row>
     <row r="242" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="243" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A243" s="41" t="s">
+      <c r="A243" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="B243" s="42"/>
-      <c r="C243" s="42"/>
-      <c r="D243" s="43"/>
-      <c r="E243" s="44" t="s">
+      <c r="B243" s="39"/>
+      <c r="C243" s="39"/>
+      <c r="D243" s="40"/>
+      <c r="E243" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="F243" s="45"/>
-      <c r="G243" s="45"/>
-      <c r="H243" s="46"/>
+      <c r="F243" s="42"/>
+      <c r="G243" s="42"/>
+      <c r="H243" s="43"/>
     </row>
     <row r="244" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A244" s="13" t="s">
@@ -11225,14 +11239,14 @@
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A245" s="38"/>
-      <c r="B245" s="39"/>
-      <c r="C245" s="39"/>
-      <c r="D245" s="39"/>
-      <c r="E245" s="39"/>
-      <c r="F245" s="39"/>
-      <c r="G245" s="39"/>
-      <c r="H245" s="40"/>
+      <c r="A245" s="44"/>
+      <c r="B245" s="45"/>
+      <c r="C245" s="45"/>
+      <c r="D245" s="45"/>
+      <c r="E245" s="45"/>
+      <c r="F245" s="45"/>
+      <c r="G245" s="45"/>
+      <c r="H245" s="46"/>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" s="17" t="str">
@@ -11733,22 +11747,15 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="E64:H64"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="E161:H161"/>
-    <mergeCell ref="A163:H163"/>
-    <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="E128:H128"/>
-    <mergeCell ref="A130:H130"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="E144:H144"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A205:D205"/>
+    <mergeCell ref="E205:H205"/>
+    <mergeCell ref="A245:H245"/>
+    <mergeCell ref="A207:H207"/>
+    <mergeCell ref="A223:D223"/>
+    <mergeCell ref="E223:H223"/>
+    <mergeCell ref="A225:H225"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="E243:H243"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="E17:H17"/>
     <mergeCell ref="A183:D183"/>
@@ -11765,15 +11772,22 @@
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A205:D205"/>
-    <mergeCell ref="E205:H205"/>
-    <mergeCell ref="A245:H245"/>
-    <mergeCell ref="A207:H207"/>
-    <mergeCell ref="A223:D223"/>
-    <mergeCell ref="E223:H223"/>
-    <mergeCell ref="A225:H225"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="E243:H243"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="E64:H64"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="E161:H161"/>
+    <mergeCell ref="A163:H163"/>
+    <mergeCell ref="A113:H113"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="E128:H128"/>
+    <mergeCell ref="A130:H130"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="E144:H144"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>